<commit_message>
Update README and Sample Data.xlsx
</commit_message>
<xml_diff>
--- a/Sample Data.xlsx
+++ b/Sample Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Programming\Python\student-topic-assigner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F40DDF71-8755-47CB-A809-05934B9FC6FB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17D4D70F-C26F-4D72-ABD9-BB9DFCAA65F6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2490" yWindow="1590" windowWidth="14310" windowHeight="12375" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9885" yWindow="2265" windowWidth="14310" windowHeight="12375" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="27">
   <si>
     <t>Name</t>
   </si>
@@ -435,7 +435,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="27" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -513,9 +513,6 @@
       <c r="C5" t="s">
         <v>17</v>
       </c>
-      <c r="D5" t="s">
-        <v>15</v>
-      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -568,9 +565,6 @@
       </c>
       <c r="C9" t="s">
         <v>14</v>
-      </c>
-      <c r="D9" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>